<commit_message>
Updated coordinate system graphic in Spreadsheet
</commit_message>
<xml_diff>
--- a/MPPG Empty Spreadsheet.xlsx
+++ b/MPPG Empty Spreadsheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smilowitz/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacqmin/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40460" windowHeight="22100" tabRatio="707" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40460" windowHeight="22100" tabRatio="707"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="20" r:id="rId1"/>
@@ -3097,6 +3097,46 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="22" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3177,6 +3217,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3184,42 +3242,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3243,6 +3265,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3267,46 +3307,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="22" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -4588,910 +4588,59 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>711574</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76573</xdr:rowOff>
+      <xdr:colOff>298823</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3676494</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>151280</xdr:rowOff>
+      <xdr:colOff>5709022</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>124013</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1"/>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="igure 2.1: Coordinate system used for measured data (courtesy of OmniP"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9496986" y="2011455"/>
-          <a:ext cx="3838979" cy="3376707"/>
-          <a:chOff x="2060472" y="1117131"/>
-          <a:chExt cx="3732524" cy="3658431"/>
+          <a:off x="9084235" y="1374589"/>
+          <a:ext cx="6284258" cy="5345953"/>
         </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2060472" y="1117131"/>
-            <a:ext cx="3732524" cy="3658431"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1"/>
-          </a:solidFill>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="3">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="2">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
-            <a:prstTxWarp prst="textNoShape">
-              <a:avLst/>
-            </a:prstTxWarp>
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="en-US"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 3"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="1980570">
-            <a:off x="3596311" y="1876877"/>
-            <a:ext cx="439112" cy="1810843"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="65000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="3">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="2">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
-            <a:prstTxWarp prst="textNoShape">
-              <a:avLst/>
-            </a:prstTxWarp>
-            <a:noAutofit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="en-US"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="5" name="Straight Connector 4"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="2983278" y="1420570"/>
-            <a:ext cx="1726922" cy="2640416"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="6" name="Straight Connector 5"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="3193319" y="2402872"/>
-            <a:ext cx="1299918" cy="712638"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="7" name="Straight Connector 6"/>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3846739" y="1595431"/>
-            <a:ext cx="0" cy="2256687"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="TextBox 7"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3360231" y="1226099"/>
-            <a:ext cx="1078184" cy="276999"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square" rtlCol="0">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="en-US"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>Y (depth)</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="TextBox 8"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2595001" y="2464167"/>
-            <a:ext cx="1233403" cy="276999"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square" rtlCol="0">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="en-US"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>X crossline</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="TextBox 9"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2115767" y="4060986"/>
-            <a:ext cx="2322648" cy="276999"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square" rtlCol="0">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="en-US"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>Z (inline with gun-target axis)</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="TextBox 10"/>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="3845620" y="3430344"/>
-            <a:ext cx="1729160" cy="461665"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr wrap="square" rtlCol="0">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle>
-            <a:defPPr>
-              <a:defRPr lang="en-US"/>
-            </a:defPPr>
-            <a:lvl1pPr marL="0" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl1pPr>
-            <a:lvl2pPr marL="457200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl2pPr>
-            <a:lvl3pPr marL="914400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl3pPr>
-            <a:lvl4pPr marL="1371600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl4pPr>
-            <a:lvl5pPr marL="1828800" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl5pPr>
-            <a:lvl6pPr marL="2286000" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl6pPr>
-            <a:lvl7pPr marL="2743200" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl7pPr>
-            <a:lvl8pPr marL="3200400" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl8pPr>
-            <a:lvl9pPr marL="3657600" algn="l" defTabSz="457200" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-              <a:defRPr sz="1800" kern="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:lvl9pPr>
-          </a:lstStyle>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>Grey is couch at home position</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6130,7 +5279,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -6522,8 +5671,8 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6547,7 +5696,7 @@
       <c r="C3" s="340" t="s">
         <v>275</v>
       </c>
-      <c r="D3" s="417" t="s">
+      <c r="D3" s="375" t="s">
         <v>276</v>
       </c>
     </row>
@@ -6558,7 +5707,7 @@
       <c r="C4" s="340">
         <v>1</v>
       </c>
-      <c r="D4" s="417"/>
+      <c r="D4" s="375"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="340" t="s">
@@ -6572,154 +5721,155 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="418" t="s">
+      <c r="A6" s="360" t="s">
         <v>280</v>
       </c>
       <c r="B6" s="217"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="418" t="s">
+      <c r="A7" s="360" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="418" t="s">
+      <c r="A8" s="360" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="419"/>
+      <c r="B8" s="361"/>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="418" t="s">
+      <c r="A9" s="360" t="s">
         <v>283</v>
       </c>
-      <c r="B9" s="419"/>
+      <c r="B9" s="361"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="418" t="s">
+      <c r="A10" s="360" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="420" t="s">
+      <c r="A12" s="362" t="s">
         <v>285</v>
       </c>
-      <c r="B12" s="421" t="s">
+      <c r="B12" s="363" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="422" t="s">
+      <c r="A13" s="364" t="s">
         <v>287</v>
       </c>
-      <c r="B13" s="423"/>
+      <c r="B13" s="365"/>
+      <c r="D13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="422" t="s">
+      <c r="A14" s="364" t="s">
         <v>288</v>
       </c>
-      <c r="B14" s="423"/>
+      <c r="B14" s="365"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="422" t="s">
+      <c r="A15" s="364" t="s">
         <v>289</v>
       </c>
-      <c r="B15" s="423"/>
+      <c r="B15" s="365"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="424" t="s">
+      <c r="A16" s="366" t="s">
         <v>290</v>
       </c>
-      <c r="B16" s="425"/>
+      <c r="B16" s="367"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="424" t="s">
+      <c r="A17" s="366" t="s">
         <v>291</v>
       </c>
-      <c r="B17" s="425"/>
+      <c r="B17" s="367"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="424" t="s">
+      <c r="A18" s="366" t="s">
         <v>292</v>
       </c>
-      <c r="B18" s="425"/>
+      <c r="B18" s="367"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="424" t="s">
+      <c r="A19" s="366" t="s">
         <v>293</v>
       </c>
-      <c r="B19" s="425"/>
+      <c r="B19" s="367"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="424" t="s">
+      <c r="A20" s="366" t="s">
         <v>294</v>
       </c>
-      <c r="B20" s="425"/>
+      <c r="B20" s="367"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="424" t="s">
+      <c r="A21" s="366" t="s">
         <v>295</v>
       </c>
-      <c r="B21" s="425"/>
+      <c r="B21" s="367"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="426" t="s">
+      <c r="A22" s="368" t="s">
         <v>296</v>
       </c>
-      <c r="B22" s="427"/>
+      <c r="B22" s="369"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="426" t="s">
+      <c r="A23" s="368" t="s">
         <v>297</v>
       </c>
-      <c r="B23" s="427"/>
+      <c r="B23" s="369"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="428" t="s">
+      <c r="A24" s="370" t="s">
         <v>298</v>
       </c>
-      <c r="B24" s="429"/>
+      <c r="B24" s="371"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="428" t="s">
+      <c r="A25" s="370" t="s">
         <v>299</v>
       </c>
-      <c r="B25" s="429"/>
+      <c r="B25" s="371"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="428" t="s">
+      <c r="A26" s="370" t="s">
         <v>300</v>
       </c>
-      <c r="B26" s="429"/>
+      <c r="B26" s="371"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="428" t="s">
+      <c r="A27" s="370" t="s">
         <v>301</v>
       </c>
-      <c r="B27" s="429"/>
+      <c r="B27" s="371"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="428" t="s">
+      <c r="A28" s="370" t="s">
         <v>302</v>
       </c>
-      <c r="B28" s="429"/>
+      <c r="B28" s="371"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="430">
+      <c r="A29" s="372">
         <v>8.1</v>
       </c>
-      <c r="B29" s="431"/>
+      <c r="B29" s="373"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="430">
+      <c r="A30" s="372">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B30" s="431"/>
+      <c r="B30" s="373"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="430">
+      <c r="A31" s="372">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B31" s="431"/>
+      <c r="B31" s="373"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6775,51 +5925,51 @@
       <c r="A4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>230</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
-      <c r="H4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="376"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
-      <c r="H5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
+      <c r="H5" s="376"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="76"/>
@@ -7427,7 +6577,7 @@
       <c r="G7" s="223"/>
       <c r="H7" s="223"/>
       <c r="I7" s="340"/>
-      <c r="J7" s="432" t="s">
+      <c r="J7" s="374" t="s">
         <v>303</v>
       </c>
     </row>
@@ -7979,25 +7129,25 @@
       <c r="A3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="360" t="s">
+      <c r="B3" s="376" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="360"/>
-      <c r="D3" s="360"/>
-      <c r="E3" s="360"/>
-      <c r="F3" s="360"/>
-      <c r="G3" s="360"/>
+      <c r="C3" s="376"/>
+      <c r="D3" s="376"/>
+      <c r="E3" s="376"/>
+      <c r="F3" s="376"/>
+      <c r="G3" s="376"/>
       <c r="J3" s="70"/>
       <c r="K3" s="70"/>
     </row>
     <row r="4" spans="1:11" s="215" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="218"/>
-      <c r="B4" s="360"/>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
+      <c r="B4" s="376"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
     </row>
     <row r="5" spans="1:11" s="70" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="73" t="s">
@@ -8021,14 +7171,14 @@
       <c r="A7" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="360" t="s">
+      <c r="B7" s="376" t="s">
         <v>224</v>
       </c>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
       <c r="H7" s="210"/>
       <c r="I7" s="210"/>
       <c r="J7" s="210"/>
@@ -8036,12 +7186,12 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="70"/>
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
       <c r="H8" s="210"/>
       <c r="I8" s="210"/>
       <c r="J8" s="210"/>
@@ -8049,12 +7199,12 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="70"/>
-      <c r="B9" s="360"/>
-      <c r="C9" s="360"/>
-      <c r="D9" s="360"/>
-      <c r="E9" s="360"/>
-      <c r="F9" s="360"/>
-      <c r="G9" s="360"/>
+      <c r="B9" s="376"/>
+      <c r="C9" s="376"/>
+      <c r="D9" s="376"/>
+      <c r="E9" s="376"/>
+      <c r="F9" s="376"/>
+      <c r="G9" s="376"/>
       <c r="H9" s="210"/>
       <c r="I9" s="210"/>
       <c r="J9" s="210"/>
@@ -8062,12 +7212,12 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="70"/>
-      <c r="B10" s="360"/>
-      <c r="C10" s="360"/>
-      <c r="D10" s="360"/>
-      <c r="E10" s="360"/>
-      <c r="F10" s="360"/>
-      <c r="G10" s="360"/>
+      <c r="B10" s="376"/>
+      <c r="C10" s="376"/>
+      <c r="D10" s="376"/>
+      <c r="E10" s="376"/>
+      <c r="F10" s="376"/>
+      <c r="G10" s="376"/>
       <c r="H10" s="210"/>
       <c r="I10" s="210"/>
       <c r="J10" s="210"/>
@@ -8075,64 +7225,64 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="70"/>
-      <c r="B11" s="360"/>
-      <c r="C11" s="360"/>
-      <c r="D11" s="360"/>
-      <c r="E11" s="360"/>
-      <c r="F11" s="360"/>
-      <c r="G11" s="360"/>
+      <c r="B11" s="376"/>
+      <c r="C11" s="376"/>
+      <c r="D11" s="376"/>
+      <c r="E11" s="376"/>
+      <c r="F11" s="376"/>
+      <c r="G11" s="376"/>
       <c r="H11" s="210"/>
       <c r="I11" s="210"/>
       <c r="J11" s="210"/>
       <c r="K11" s="210"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="360"/>
-      <c r="C12" s="360"/>
-      <c r="D12" s="360"/>
-      <c r="E12" s="360"/>
-      <c r="F12" s="360"/>
-      <c r="G12" s="360"/>
+      <c r="B12" s="376"/>
+      <c r="C12" s="376"/>
+      <c r="D12" s="376"/>
+      <c r="E12" s="376"/>
+      <c r="F12" s="376"/>
+      <c r="G12" s="376"/>
     </row>
     <row r="13" spans="1:11" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="360"/>
-      <c r="C13" s="360"/>
-      <c r="D13" s="360"/>
-      <c r="E13" s="360"/>
-      <c r="F13" s="360"/>
-      <c r="G13" s="360"/>
+      <c r="B13" s="376"/>
+      <c r="C13" s="376"/>
+      <c r="D13" s="376"/>
+      <c r="E13" s="376"/>
+      <c r="F13" s="376"/>
+      <c r="G13" s="376"/>
     </row>
     <row r="14" spans="1:11" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="360"/>
-      <c r="C14" s="360"/>
-      <c r="D14" s="360"/>
-      <c r="E14" s="360"/>
-      <c r="F14" s="360"/>
-      <c r="G14" s="360"/>
+      <c r="B14" s="376"/>
+      <c r="C14" s="376"/>
+      <c r="D14" s="376"/>
+      <c r="E14" s="376"/>
+      <c r="F14" s="376"/>
+      <c r="G14" s="376"/>
     </row>
     <row r="15" spans="1:11" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="360"/>
-      <c r="C15" s="360"/>
-      <c r="D15" s="360"/>
-      <c r="E15" s="360"/>
-      <c r="F15" s="360"/>
-      <c r="G15" s="360"/>
+      <c r="B15" s="376"/>
+      <c r="C15" s="376"/>
+      <c r="D15" s="376"/>
+      <c r="E15" s="376"/>
+      <c r="F15" s="376"/>
+      <c r="G15" s="376"/>
     </row>
     <row r="16" spans="1:11" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="360"/>
-      <c r="C16" s="360"/>
-      <c r="D16" s="360"/>
-      <c r="E16" s="360"/>
-      <c r="F16" s="360"/>
-      <c r="G16" s="360"/>
+      <c r="B16" s="376"/>
+      <c r="C16" s="376"/>
+      <c r="D16" s="376"/>
+      <c r="E16" s="376"/>
+      <c r="F16" s="376"/>
+      <c r="G16" s="376"/>
     </row>
     <row r="17" spans="1:23" s="70" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="360"/>
-      <c r="C17" s="360"/>
-      <c r="D17" s="360"/>
-      <c r="E17" s="360"/>
-      <c r="F17" s="360"/>
-      <c r="G17" s="360"/>
+      <c r="B17" s="376"/>
+      <c r="C17" s="376"/>
+      <c r="D17" s="376"/>
+      <c r="E17" s="376"/>
+      <c r="F17" s="376"/>
+      <c r="G17" s="376"/>
     </row>
     <row r="19" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="73" t="s">
@@ -8157,35 +7307,35 @@
       <c r="B20" s="73"/>
       <c r="C20" s="73"/>
       <c r="D20" s="73"/>
-      <c r="E20" s="390" t="s">
+      <c r="E20" s="403" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="391"/>
-      <c r="G20" s="391"/>
-      <c r="H20" s="391"/>
-      <c r="I20" s="391"/>
-      <c r="J20" s="391"/>
-      <c r="K20" s="392"/>
-      <c r="L20" s="393" t="s">
+      <c r="F20" s="404"/>
+      <c r="G20" s="404"/>
+      <c r="H20" s="404"/>
+      <c r="I20" s="404"/>
+      <c r="J20" s="404"/>
+      <c r="K20" s="405"/>
+      <c r="L20" s="406" t="s">
         <v>69</v>
       </c>
-      <c r="M20" s="394"/>
-      <c r="N20" s="395"/>
-      <c r="O20" s="387" t="s">
+      <c r="M20" s="407"/>
+      <c r="N20" s="408"/>
+      <c r="O20" s="409" t="s">
         <v>171</v>
       </c>
-      <c r="P20" s="388"/>
-      <c r="Q20" s="389"/>
-      <c r="R20" s="387" t="s">
+      <c r="P20" s="410"/>
+      <c r="Q20" s="411"/>
+      <c r="R20" s="409" t="s">
         <v>172</v>
       </c>
-      <c r="S20" s="388"/>
-      <c r="T20" s="389"/>
-      <c r="U20" s="387" t="s">
+      <c r="S20" s="410"/>
+      <c r="T20" s="411"/>
+      <c r="U20" s="409" t="s">
         <v>170</v>
       </c>
-      <c r="V20" s="388"/>
-      <c r="W20" s="389"/>
+      <c r="V20" s="410"/>
+      <c r="W20" s="411"/>
     </row>
     <row r="21" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="80" t="s">
@@ -9138,39 +8288,39 @@
       <c r="A3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="360" t="s">
+      <c r="B3" s="376" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="360"/>
-      <c r="D3" s="360"/>
-      <c r="E3" s="360"/>
-      <c r="F3" s="360"/>
+      <c r="C3" s="376"/>
+      <c r="D3" s="376"/>
+      <c r="E3" s="376"/>
+      <c r="F3" s="376"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="73"/>
-      <c r="B4" s="360"/>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
+      <c r="B4" s="376"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
       <c r="G4" s="210"/>
       <c r="H4" s="210"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
       <c r="G5" s="210"/>
       <c r="H5" s="210"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
       <c r="G6" s="210"/>
       <c r="H6" s="210"/>
     </row>
@@ -9275,50 +8425,50 @@
       <c r="A17" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="M17" s="409" t="s">
+      <c r="M17" s="425" t="s">
         <v>162</v>
       </c>
-      <c r="N17" s="409"/>
-      <c r="O17" s="409"/>
-      <c r="P17" s="409"/>
-      <c r="Q17" s="409"/>
-      <c r="R17" s="409"/>
-      <c r="S17" s="409"/>
-      <c r="T17" s="409"/>
+      <c r="N17" s="425"/>
+      <c r="O17" s="425"/>
+      <c r="P17" s="425"/>
+      <c r="Q17" s="425"/>
+      <c r="R17" s="425"/>
+      <c r="S17" s="425"/>
+      <c r="T17" s="425"/>
     </row>
     <row r="18" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="73"/>
       <c r="B18" s="73"/>
       <c r="C18" s="73"/>
       <c r="D18" s="73"/>
-      <c r="E18" s="390" t="s">
+      <c r="E18" s="403" t="s">
         <v>147</v>
       </c>
-      <c r="F18" s="392"/>
-      <c r="G18" s="393" t="s">
+      <c r="F18" s="405"/>
+      <c r="G18" s="406" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="394"/>
-      <c r="I18" s="395"/>
-      <c r="J18" s="387" t="s">
+      <c r="H18" s="407"/>
+      <c r="I18" s="408"/>
+      <c r="J18" s="409" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="388"/>
-      <c r="L18" s="389"/>
-      <c r="M18" s="390" t="s">
+      <c r="K18" s="410"/>
+      <c r="L18" s="411"/>
+      <c r="M18" s="403" t="s">
         <v>147</v>
       </c>
-      <c r="N18" s="392"/>
-      <c r="O18" s="393" t="s">
+      <c r="N18" s="405"/>
+      <c r="O18" s="406" t="s">
         <v>69</v>
       </c>
-      <c r="P18" s="394"/>
-      <c r="Q18" s="395"/>
-      <c r="R18" s="387" t="s">
+      <c r="P18" s="407"/>
+      <c r="Q18" s="408"/>
+      <c r="R18" s="409" t="s">
         <v>70</v>
       </c>
-      <c r="S18" s="388"/>
-      <c r="T18" s="389"/>
+      <c r="S18" s="410"/>
+      <c r="T18" s="411"/>
     </row>
     <row r="19" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="80" t="s">
@@ -9936,45 +9086,45 @@
     </row>
     <row r="28" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C29" s="378" t="s">
+      <c r="C29" s="394" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="379"/>
-      <c r="E29" s="379"/>
-      <c r="F29" s="379"/>
-      <c r="G29" s="380"/>
-      <c r="H29" s="381" t="s">
+      <c r="D29" s="395"/>
+      <c r="E29" s="395"/>
+      <c r="F29" s="395"/>
+      <c r="G29" s="396"/>
+      <c r="H29" s="397" t="s">
         <v>70</v>
       </c>
-      <c r="I29" s="382"/>
-      <c r="J29" s="382"/>
-      <c r="K29" s="382"/>
-      <c r="L29" s="383"/>
+      <c r="I29" s="398"/>
+      <c r="J29" s="398"/>
+      <c r="K29" s="398"/>
+      <c r="L29" s="399"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="371" t="s">
+      <c r="C30" s="387" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="372"/>
-      <c r="E30" s="372"/>
+      <c r="D30" s="388"/>
+      <c r="E30" s="388"/>
       <c r="F30" s="203" t="s">
         <v>83</v>
       </c>
-      <c r="G30" s="373" t="s">
+      <c r="G30" s="389" t="s">
         <v>82</v>
       </c>
-      <c r="H30" s="384" t="s">
+      <c r="H30" s="400" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="385"/>
-      <c r="J30" s="385"/>
+      <c r="I30" s="401"/>
+      <c r="J30" s="401"/>
       <c r="K30" s="202" t="s">
         <v>83</v>
       </c>
-      <c r="L30" s="386" t="s">
+      <c r="L30" s="402" t="s">
         <v>82</v>
       </c>
     </row>
@@ -9994,7 +9144,7 @@
       <c r="F31" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="G31" s="374"/>
+      <c r="G31" s="390"/>
       <c r="H31" s="154" t="s">
         <v>81</v>
       </c>
@@ -10007,7 +9157,7 @@
       <c r="K31" s="151" t="s">
         <v>89</v>
       </c>
-      <c r="L31" s="386"/>
+      <c r="L31" s="402"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="142">
@@ -10082,63 +9232,69 @@
       <c r="L35" s="198"/>
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="360" t="s">
+      <c r="A37" s="376" t="s">
         <v>179</v>
       </c>
-      <c r="B37" s="360"/>
-      <c r="C37" s="360"/>
-      <c r="D37" s="360"/>
-      <c r="E37" s="360"/>
-      <c r="F37" s="360"/>
-      <c r="G37" s="360"/>
+      <c r="B37" s="376"/>
+      <c r="C37" s="376"/>
+      <c r="D37" s="376"/>
+      <c r="E37" s="376"/>
+      <c r="F37" s="376"/>
+      <c r="G37" s="376"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="360"/>
-      <c r="B38" s="360"/>
-      <c r="C38" s="360"/>
-      <c r="D38" s="360"/>
-      <c r="E38" s="360"/>
-      <c r="F38" s="360"/>
-      <c r="G38" s="360"/>
+      <c r="A38" s="376"/>
+      <c r="B38" s="376"/>
+      <c r="C38" s="376"/>
+      <c r="D38" s="376"/>
+      <c r="E38" s="376"/>
+      <c r="F38" s="376"/>
+      <c r="G38" s="376"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="360"/>
-      <c r="B39" s="360"/>
-      <c r="C39" s="360"/>
-      <c r="D39" s="360"/>
-      <c r="E39" s="360"/>
-      <c r="F39" s="360"/>
-      <c r="G39" s="360"/>
+      <c r="A39" s="376"/>
+      <c r="B39" s="376"/>
+      <c r="C39" s="376"/>
+      <c r="D39" s="376"/>
+      <c r="E39" s="376"/>
+      <c r="F39" s="376"/>
+      <c r="G39" s="376"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="360"/>
-      <c r="B40" s="360"/>
-      <c r="C40" s="360"/>
-      <c r="D40" s="360"/>
-      <c r="E40" s="360"/>
-      <c r="F40" s="360"/>
-      <c r="G40" s="360"/>
+      <c r="A40" s="376"/>
+      <c r="B40" s="376"/>
+      <c r="C40" s="376"/>
+      <c r="D40" s="376"/>
+      <c r="E40" s="376"/>
+      <c r="F40" s="376"/>
+      <c r="G40" s="376"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="360"/>
-      <c r="B41" s="360"/>
-      <c r="C41" s="360"/>
-      <c r="D41" s="360"/>
-      <c r="E41" s="360"/>
-      <c r="F41" s="360"/>
-      <c r="G41" s="360"/>
+      <c r="A41" s="376"/>
+      <c r="B41" s="376"/>
+      <c r="C41" s="376"/>
+      <c r="D41" s="376"/>
+      <c r="E41" s="376"/>
+      <c r="F41" s="376"/>
+      <c r="G41" s="376"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="360"/>
-      <c r="B42" s="360"/>
-      <c r="C42" s="360"/>
-      <c r="D42" s="360"/>
-      <c r="E42" s="360"/>
-      <c r="F42" s="360"/>
-      <c r="G42" s="360"/>
+      <c r="A42" s="376"/>
+      <c r="B42" s="376"/>
+      <c r="C42" s="376"/>
+      <c r="D42" s="376"/>
+      <c r="E42" s="376"/>
+      <c r="F42" s="376"/>
+      <c r="G42" s="376"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="M17:T17"/>
+    <mergeCell ref="B3:F6"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="R18:T18"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="H29:L29"/>
     <mergeCell ref="A37:G42"/>
@@ -10148,12 +9304,6 @@
     <mergeCell ref="G30:G31"/>
     <mergeCell ref="H30:J30"/>
     <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M17:T17"/>
-    <mergeCell ref="B3:F6"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="R18:T18"/>
   </mergeCells>
   <conditionalFormatting sqref="C32:L35">
     <cfRule type="containsBlanks" dxfId="55" priority="29">
@@ -10272,37 +9422,37 @@
       <c r="A3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="360" t="s">
+      <c r="B3" s="376" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="360"/>
-      <c r="D3" s="360"/>
-      <c r="E3" s="360"/>
-      <c r="F3" s="360"/>
+      <c r="C3" s="376"/>
+      <c r="D3" s="376"/>
+      <c r="E3" s="376"/>
+      <c r="F3" s="376"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="73"/>
-      <c r="B4" s="360"/>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
+      <c r="B4" s="376"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="70"/>
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="70"/>
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -10310,18 +9460,18 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="410" t="s">
+      <c r="A9" s="426" t="s">
         <v>175</v>
       </c>
-      <c r="B9" s="410"/>
-      <c r="C9" s="410"/>
-      <c r="D9" s="410"/>
-      <c r="E9" s="410"/>
-      <c r="F9" s="410"/>
-      <c r="G9" s="410"/>
-      <c r="H9" s="410"/>
-      <c r="I9" s="410"/>
-      <c r="J9" s="410"/>
+      <c r="B9" s="426"/>
+      <c r="C9" s="426"/>
+      <c r="D9" s="426"/>
+      <c r="E9" s="426"/>
+      <c r="F9" s="426"/>
+      <c r="G9" s="426"/>
+      <c r="H9" s="426"/>
+      <c r="I9" s="426"/>
+      <c r="J9" s="426"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10376,37 +9526,37 @@
       <c r="A3" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="360" t="s">
+      <c r="B3" s="376" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="360"/>
-      <c r="D3" s="360"/>
-      <c r="E3" s="360"/>
-      <c r="F3" s="360"/>
+      <c r="C3" s="376"/>
+      <c r="D3" s="376"/>
+      <c r="E3" s="376"/>
+      <c r="F3" s="376"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="73"/>
-      <c r="B4" s="360"/>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
+      <c r="B4" s="376"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="70"/>
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="70"/>
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="70"/>
@@ -10510,51 +9660,51 @@
       <c r="A6" s="218" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="360" t="s">
+      <c r="B6" s="376" t="s">
         <v>183</v>
       </c>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="360"/>
-      <c r="C9" s="360"/>
-      <c r="D9" s="360"/>
-      <c r="E9" s="360"/>
-      <c r="F9" s="360"/>
-      <c r="G9" s="360"/>
-      <c r="H9" s="360"/>
+      <c r="B9" s="376"/>
+      <c r="C9" s="376"/>
+      <c r="D9" s="376"/>
+      <c r="E9" s="376"/>
+      <c r="F9" s="376"/>
+      <c r="G9" s="376"/>
+      <c r="H9" s="376"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="360"/>
-      <c r="C10" s="360"/>
-      <c r="D10" s="360"/>
-      <c r="E10" s="360"/>
-      <c r="F10" s="360"/>
-      <c r="G10" s="360"/>
-      <c r="H10" s="360"/>
+      <c r="B10" s="376"/>
+      <c r="C10" s="376"/>
+      <c r="D10" s="376"/>
+      <c r="E10" s="376"/>
+      <c r="F10" s="376"/>
+      <c r="G10" s="376"/>
+      <c r="H10" s="376"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="222"/>
@@ -10631,46 +9781,46 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="413" t="s">
+      <c r="A19" s="429" t="s">
         <v>187</v>
       </c>
-      <c r="B19" s="413"/>
-      <c r="C19" s="413"/>
-      <c r="D19" s="413"/>
-      <c r="E19" s="413"/>
-      <c r="F19" s="413"/>
-      <c r="G19" s="413"/>
-      <c r="H19" s="413"/>
-      <c r="I19" s="413"/>
-      <c r="J19" s="413"/>
-      <c r="K19" s="413"/>
-      <c r="L19" s="413"/>
+      <c r="B19" s="429"/>
+      <c r="C19" s="429"/>
+      <c r="D19" s="429"/>
+      <c r="E19" s="429"/>
+      <c r="F19" s="429"/>
+      <c r="G19" s="429"/>
+      <c r="H19" s="429"/>
+      <c r="I19" s="429"/>
+      <c r="J19" s="429"/>
+      <c r="K19" s="429"/>
+      <c r="L19" s="429"/>
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="411" t="s">
+      <c r="A20" s="427" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="411" t="s">
+      <c r="B20" s="427" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="412" t="s">
+      <c r="C20" s="428" t="s">
         <v>193</v>
       </c>
-      <c r="D20" s="412"/>
-      <c r="E20" s="412"/>
-      <c r="F20" s="412"/>
-      <c r="G20" s="412"/>
-      <c r="H20" s="412" t="s">
+      <c r="D20" s="428"/>
+      <c r="E20" s="428"/>
+      <c r="F20" s="428"/>
+      <c r="G20" s="428"/>
+      <c r="H20" s="428" t="s">
         <v>194</v>
       </c>
-      <c r="I20" s="412"/>
-      <c r="J20" s="412"/>
-      <c r="K20" s="412"/>
-      <c r="L20" s="412"/>
+      <c r="I20" s="428"/>
+      <c r="J20" s="428"/>
+      <c r="K20" s="428"/>
+      <c r="L20" s="428"/>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="411"/>
-      <c r="B21" s="411"/>
+      <c r="A21" s="427"/>
+      <c r="B21" s="427"/>
       <c r="C21" s="286" t="s">
         <v>189</v>
       </c>
@@ -10979,55 +10129,55 @@
       <c r="A4" s="218" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>207</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
-      <c r="H4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="376"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="215"/>
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
-      <c r="H5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
+      <c r="H5" s="376"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="215"/>
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="215"/>
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="215"/>
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="218" t="s">
@@ -11180,18 +10330,18 @@
       <c r="B22" s="73"/>
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
-      <c r="E22" s="368" t="s">
+      <c r="E22" s="384" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="369"/>
-      <c r="G22" s="369"/>
-      <c r="H22" s="369"/>
-      <c r="I22" s="370"/>
-      <c r="J22" s="375" t="s">
+      <c r="F22" s="385"/>
+      <c r="G22" s="385"/>
+      <c r="H22" s="385"/>
+      <c r="I22" s="386"/>
+      <c r="J22" s="391" t="s">
         <v>181</v>
       </c>
-      <c r="K22" s="376"/>
-      <c r="L22" s="377"/>
+      <c r="K22" s="392"/>
+      <c r="L22" s="393"/>
     </row>
     <row r="23" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="313" t="s">
@@ -11745,28 +10895,28 @@
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="215"/>
       <c r="B40" s="215"/>
-      <c r="C40" s="378" t="s">
+      <c r="C40" s="394" t="s">
         <v>196</v>
       </c>
-      <c r="D40" s="379"/>
-      <c r="E40" s="379"/>
-      <c r="F40" s="379"/>
-      <c r="G40" s="414"/>
+      <c r="D40" s="395"/>
+      <c r="E40" s="395"/>
+      <c r="F40" s="395"/>
+      <c r="G40" s="430"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="264" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="215"/>
-      <c r="C41" s="371" t="s">
+      <c r="C41" s="387" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="372"/>
-      <c r="E41" s="372" t="s">
+      <c r="D41" s="388"/>
+      <c r="E41" s="388" t="s">
         <v>83</v>
       </c>
-      <c r="F41" s="372"/>
-      <c r="G41" s="406" t="s">
+      <c r="F41" s="388"/>
+      <c r="G41" s="416" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11787,7 +10937,7 @@
       <c r="F42" s="282" t="s">
         <v>201</v>
       </c>
-      <c r="G42" s="406"/>
+      <c r="G42" s="416"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="316" t="s">
@@ -11858,28 +11008,28 @@
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="215"/>
       <c r="B49" s="215"/>
-      <c r="C49" s="378" t="s">
+      <c r="C49" s="394" t="s">
         <v>196</v>
       </c>
-      <c r="D49" s="379"/>
-      <c r="E49" s="379"/>
-      <c r="F49" s="379"/>
-      <c r="G49" s="414"/>
+      <c r="D49" s="395"/>
+      <c r="E49" s="395"/>
+      <c r="F49" s="395"/>
+      <c r="G49" s="430"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="264" t="s">
         <v>80</v>
       </c>
       <c r="B50" s="215"/>
-      <c r="C50" s="371" t="s">
+      <c r="C50" s="387" t="s">
         <v>84</v>
       </c>
-      <c r="D50" s="372"/>
-      <c r="E50" s="372" t="s">
+      <c r="D50" s="388"/>
+      <c r="E50" s="388" t="s">
         <v>83</v>
       </c>
-      <c r="F50" s="372"/>
-      <c r="G50" s="406" t="s">
+      <c r="F50" s="388"/>
+      <c r="G50" s="416" t="s">
         <v>82</v>
       </c>
     </row>
@@ -11900,7 +11050,7 @@
       <c r="F51" s="282" t="s">
         <v>201</v>
       </c>
-      <c r="G51" s="406"/>
+      <c r="G51" s="416"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="316" t="s">
@@ -11969,17 +11119,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B4:H8"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="G41:G42"/>
     <mergeCell ref="C49:G49"/>
     <mergeCell ref="G50:G51"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B4:H8"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="G41:G42"/>
   </mergeCells>
   <conditionalFormatting sqref="C43:G43 C45:G47">
     <cfRule type="containsBlanks" dxfId="30" priority="10">
@@ -12070,46 +11220,46 @@
       <c r="A4" s="218" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="218" t="s">
@@ -12224,18 +11374,18 @@
       <c r="E22" s="218"/>
       <c r="F22" s="218"/>
       <c r="G22" s="218"/>
-      <c r="H22" s="368" t="s">
+      <c r="H22" s="384" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="369"/>
-      <c r="J22" s="369"/>
-      <c r="K22" s="369"/>
-      <c r="L22" s="370"/>
-      <c r="M22" s="375" t="s">
+      <c r="I22" s="385"/>
+      <c r="J22" s="385"/>
+      <c r="K22" s="385"/>
+      <c r="L22" s="386"/>
+      <c r="M22" s="391" t="s">
         <v>181</v>
       </c>
-      <c r="N22" s="376"/>
-      <c r="O22" s="377"/>
+      <c r="N22" s="392"/>
+      <c r="O22" s="393"/>
     </row>
     <row r="23" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="310" t="s">
@@ -12715,31 +11865,31 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="415" t="s">
+      <c r="C35" s="431" t="s">
         <v>196</v>
       </c>
-      <c r="D35" s="416"/>
-      <c r="E35" s="416"/>
-      <c r="F35" s="416"/>
-      <c r="G35" s="416"/>
-      <c r="H35" s="416"/>
+      <c r="D35" s="432"/>
+      <c r="E35" s="432"/>
+      <c r="F35" s="432"/>
+      <c r="G35" s="432"/>
+      <c r="H35" s="432"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="264" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="403" t="s">
+      <c r="C36" s="413" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="404"/>
-      <c r="E36" s="404" t="s">
+      <c r="D36" s="414"/>
+      <c r="E36" s="414" t="s">
         <v>83</v>
       </c>
-      <c r="F36" s="404"/>
-      <c r="G36" s="404" t="s">
+      <c r="F36" s="414"/>
+      <c r="G36" s="414" t="s">
         <v>82</v>
       </c>
-      <c r="H36" s="405" t="s">
+      <c r="H36" s="415" t="s">
         <v>143</v>
       </c>
     </row>
@@ -12759,8 +11909,8 @@
       <c r="F37" s="282" t="s">
         <v>201</v>
       </c>
-      <c r="G37" s="372"/>
-      <c r="H37" s="406"/>
+      <c r="G37" s="388"/>
+      <c r="H37" s="416"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="265" t="s">
@@ -12899,8 +12049,8 @@
   </sheetPr>
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12931,46 +12081,46 @@
       <c r="A4" s="218" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>216</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
     </row>
     <row r="5" spans="1:10" s="215" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
     </row>
     <row r="6" spans="1:10" s="215" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
     </row>
     <row r="7" spans="1:10" s="215" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
     </row>
     <row r="8" spans="1:10" s="215" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
     </row>
     <row r="9" spans="1:10" s="215" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="218" t="s">
@@ -13047,19 +12197,19 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="334"/>
-      <c r="B16" s="412" t="s">
+      <c r="B16" s="428" t="s">
         <v>218</v>
       </c>
-      <c r="C16" s="412"/>
-      <c r="D16" s="412"/>
-      <c r="E16" s="412"/>
-      <c r="F16" s="412"/>
-      <c r="G16" s="412"/>
-      <c r="H16" s="372" t="s">
+      <c r="C16" s="428"/>
+      <c r="D16" s="428"/>
+      <c r="E16" s="428"/>
+      <c r="F16" s="428"/>
+      <c r="G16" s="428"/>
+      <c r="H16" s="388" t="s">
         <v>196</v>
       </c>
-      <c r="I16" s="372"/>
-      <c r="J16" s="372"/>
+      <c r="I16" s="388"/>
+      <c r="J16" s="388"/>
     </row>
     <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="335" t="s">
@@ -13247,19 +12397,19 @@
     </row>
     <row r="24" spans="1:10" s="215" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="334"/>
-      <c r="B24" s="412" t="s">
+      <c r="B24" s="428" t="s">
         <v>219</v>
       </c>
-      <c r="C24" s="412"/>
-      <c r="D24" s="412"/>
-      <c r="E24" s="412"/>
-      <c r="F24" s="412"/>
-      <c r="G24" s="412"/>
-      <c r="H24" s="372" t="s">
+      <c r="C24" s="428"/>
+      <c r="D24" s="428"/>
+      <c r="E24" s="428"/>
+      <c r="F24" s="428"/>
+      <c r="G24" s="428"/>
+      <c r="H24" s="388" t="s">
         <v>196</v>
       </c>
-      <c r="I24" s="372"/>
-      <c r="J24" s="372"/>
+      <c r="I24" s="388"/>
+      <c r="J24" s="388"/>
     </row>
     <row r="25" spans="1:10" s="215" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="335" t="s">
@@ -13447,19 +12597,19 @@
     </row>
     <row r="32" spans="1:10" s="215" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="334"/>
-      <c r="B32" s="412" t="s">
+      <c r="B32" s="428" t="s">
         <v>220</v>
       </c>
-      <c r="C32" s="412"/>
-      <c r="D32" s="412"/>
-      <c r="E32" s="412"/>
-      <c r="F32" s="412"/>
-      <c r="G32" s="412"/>
-      <c r="H32" s="372" t="s">
+      <c r="C32" s="428"/>
+      <c r="D32" s="428"/>
+      <c r="E32" s="428"/>
+      <c r="F32" s="428"/>
+      <c r="G32" s="428"/>
+      <c r="H32" s="388" t="s">
         <v>196</v>
       </c>
-      <c r="I32" s="372"/>
-      <c r="J32" s="372"/>
+      <c r="I32" s="388"/>
+      <c r="J32" s="388"/>
     </row>
     <row r="33" spans="1:10" s="215" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="335" t="s">
@@ -13869,33 +13019,33 @@
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="360" t="s">
+      <c r="B6" s="376" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -13976,51 +13126,51 @@
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="360" t="s">
+      <c r="B6" s="376" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="360"/>
-      <c r="C9" s="360"/>
-      <c r="D9" s="360"/>
-      <c r="E9" s="360"/>
-      <c r="F9" s="360"/>
-      <c r="G9" s="360"/>
-      <c r="H9" s="360"/>
+      <c r="B9" s="376"/>
+      <c r="C9" s="376"/>
+      <c r="D9" s="376"/>
+      <c r="E9" s="376"/>
+      <c r="F9" s="376"/>
+      <c r="G9" s="376"/>
+      <c r="H9" s="376"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="360"/>
-      <c r="C10" s="360"/>
-      <c r="D10" s="360"/>
-      <c r="E10" s="360"/>
-      <c r="F10" s="360"/>
-      <c r="G10" s="360"/>
-      <c r="H10" s="360"/>
+      <c r="B10" s="376"/>
+      <c r="C10" s="376"/>
+      <c r="D10" s="376"/>
+      <c r="E10" s="376"/>
+      <c r="F10" s="376"/>
+      <c r="G10" s="376"/>
+      <c r="H10" s="376"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="22"/>
@@ -14100,38 +13250,38 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="363" t="s">
+      <c r="C18" s="379" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="363"/>
-      <c r="E18" s="363"/>
-      <c r="F18" s="363"/>
-      <c r="G18" s="363"/>
-      <c r="H18" s="363"/>
-      <c r="I18" s="363"/>
-      <c r="J18" s="363"/>
-      <c r="K18" s="363"/>
-      <c r="L18" s="363"/>
+      <c r="D18" s="379"/>
+      <c r="E18" s="379"/>
+      <c r="F18" s="379"/>
+      <c r="G18" s="379"/>
+      <c r="H18" s="379"/>
+      <c r="I18" s="379"/>
+      <c r="J18" s="379"/>
+      <c r="K18" s="379"/>
+      <c r="L18" s="379"/>
     </row>
     <row r="19" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="364" t="s">
+      <c r="C19" s="380" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="364"/>
-      <c r="E19" s="364"/>
-      <c r="F19" s="364" t="s">
+      <c r="D19" s="380"/>
+      <c r="E19" s="380"/>
+      <c r="F19" s="380" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="364"/>
-      <c r="H19" s="364"/>
-      <c r="I19" s="364" t="s">
+      <c r="G19" s="380"/>
+      <c r="H19" s="380"/>
+      <c r="I19" s="380" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="364"/>
-      <c r="K19" s="364"/>
-      <c r="L19" s="364"/>
+      <c r="J19" s="380"/>
+      <c r="K19" s="380"/>
+      <c r="L19" s="380"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
@@ -14340,38 +13490,38 @@
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="361" t="s">
+      <c r="C26" s="377" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="361"/>
-      <c r="E26" s="361"/>
-      <c r="F26" s="361"/>
-      <c r="G26" s="361"/>
-      <c r="H26" s="361"/>
-      <c r="I26" s="361"/>
-      <c r="J26" s="361"/>
-      <c r="K26" s="361"/>
-      <c r="L26" s="361"/>
+      <c r="D26" s="377"/>
+      <c r="E26" s="377"/>
+      <c r="F26" s="377"/>
+      <c r="G26" s="377"/>
+      <c r="H26" s="377"/>
+      <c r="I26" s="377"/>
+      <c r="J26" s="377"/>
+      <c r="K26" s="377"/>
+      <c r="L26" s="377"/>
     </row>
     <row r="27" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="362" t="s">
+      <c r="C27" s="378" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="362"/>
-      <c r="E27" s="362"/>
-      <c r="F27" s="362" t="s">
+      <c r="D27" s="378"/>
+      <c r="E27" s="378"/>
+      <c r="F27" s="378" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="362"/>
-      <c r="H27" s="362"/>
-      <c r="I27" s="362" t="s">
+      <c r="G27" s="378"/>
+      <c r="H27" s="378"/>
+      <c r="I27" s="378" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="362"/>
-      <c r="K27" s="362"/>
-      <c r="L27" s="362"/>
+      <c r="J27" s="378"/>
+      <c r="K27" s="378"/>
+      <c r="L27" s="378"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
@@ -14640,33 +13790,33 @@
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="360" t="s">
+      <c r="B6" s="376" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
@@ -14752,51 +13902,51 @@
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
-      <c r="H4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="376"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
-      <c r="H5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
+      <c r="H5" s="376"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="22"/>
@@ -14905,23 +14055,23 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="368" t="s">
+      <c r="E20" s="384" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="369"/>
-      <c r="G20" s="369"/>
-      <c r="H20" s="369"/>
-      <c r="I20" s="370"/>
-      <c r="J20" s="375" t="s">
+      <c r="F20" s="385"/>
+      <c r="G20" s="385"/>
+      <c r="H20" s="385"/>
+      <c r="I20" s="386"/>
+      <c r="J20" s="391" t="s">
         <v>69</v>
       </c>
-      <c r="K20" s="376"/>
-      <c r="L20" s="377"/>
-      <c r="M20" s="365" t="s">
+      <c r="K20" s="392"/>
+      <c r="L20" s="393"/>
+      <c r="M20" s="381" t="s">
         <v>70</v>
       </c>
-      <c r="N20" s="366"/>
-      <c r="O20" s="367"/>
+      <c r="N20" s="382"/>
+      <c r="O20" s="383"/>
     </row>
     <row r="21" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
@@ -15316,45 +14466,45 @@
     </row>
     <row r="30" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C31" s="378" t="s">
+      <c r="C31" s="394" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="379"/>
-      <c r="E31" s="379"/>
-      <c r="F31" s="379"/>
-      <c r="G31" s="380"/>
-      <c r="H31" s="381" t="s">
+      <c r="D31" s="395"/>
+      <c r="E31" s="395"/>
+      <c r="F31" s="395"/>
+      <c r="G31" s="396"/>
+      <c r="H31" s="397" t="s">
         <v>70</v>
       </c>
-      <c r="I31" s="382"/>
-      <c r="J31" s="382"/>
-      <c r="K31" s="382"/>
-      <c r="L31" s="383"/>
+      <c r="I31" s="398"/>
+      <c r="J31" s="398"/>
+      <c r="K31" s="398"/>
+      <c r="L31" s="399"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="371" t="s">
+      <c r="C32" s="387" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="372"/>
-      <c r="E32" s="372"/>
+      <c r="D32" s="388"/>
+      <c r="E32" s="388"/>
       <c r="F32" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="G32" s="373" t="s">
+      <c r="G32" s="389" t="s">
         <v>82</v>
       </c>
-      <c r="H32" s="384" t="s">
+      <c r="H32" s="400" t="s">
         <v>84</v>
       </c>
-      <c r="I32" s="385"/>
-      <c r="J32" s="385"/>
+      <c r="I32" s="401"/>
+      <c r="J32" s="401"/>
       <c r="K32" s="150" t="s">
         <v>83</v>
       </c>
-      <c r="L32" s="386" t="s">
+      <c r="L32" s="402" t="s">
         <v>82</v>
       </c>
     </row>
@@ -15374,7 +14524,7 @@
       <c r="F33" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="374"/>
+      <c r="G33" s="390"/>
       <c r="H33" s="154" t="s">
         <v>81</v>
       </c>
@@ -15387,7 +14537,7 @@
       <c r="K33" s="151" t="s">
         <v>89</v>
       </c>
-      <c r="L33" s="386"/>
+      <c r="L33" s="402"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="142" t="s">
@@ -15568,51 +14718,51 @@
       <c r="A4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
-      <c r="H4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="376"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
-      <c r="H5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
+      <c r="H5" s="376"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="76"/>
@@ -15721,23 +14871,23 @@
       <c r="B20" s="73"/>
       <c r="C20" s="73"/>
       <c r="D20" s="73"/>
-      <c r="E20" s="368" t="s">
+      <c r="E20" s="384" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="369"/>
-      <c r="G20" s="369"/>
-      <c r="H20" s="369"/>
-      <c r="I20" s="370"/>
-      <c r="J20" s="375" t="s">
+      <c r="F20" s="385"/>
+      <c r="G20" s="385"/>
+      <c r="H20" s="385"/>
+      <c r="I20" s="386"/>
+      <c r="J20" s="391" t="s">
         <v>69</v>
       </c>
-      <c r="K20" s="376"/>
-      <c r="L20" s="377"/>
-      <c r="M20" s="365" t="s">
+      <c r="K20" s="392"/>
+      <c r="L20" s="393"/>
+      <c r="M20" s="381" t="s">
         <v>70</v>
       </c>
-      <c r="N20" s="366"/>
-      <c r="O20" s="367"/>
+      <c r="N20" s="382"/>
+      <c r="O20" s="383"/>
     </row>
     <row r="21" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="80" t="s">
@@ -16195,45 +15345,45 @@
     </row>
     <row r="31" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C32" s="378" t="s">
+      <c r="C32" s="394" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="379"/>
-      <c r="E32" s="379"/>
-      <c r="F32" s="379"/>
-      <c r="G32" s="380"/>
-      <c r="H32" s="381" t="s">
+      <c r="D32" s="395"/>
+      <c r="E32" s="395"/>
+      <c r="F32" s="395"/>
+      <c r="G32" s="396"/>
+      <c r="H32" s="397" t="s">
         <v>70</v>
       </c>
-      <c r="I32" s="382"/>
-      <c r="J32" s="382"/>
-      <c r="K32" s="382"/>
-      <c r="L32" s="383"/>
+      <c r="I32" s="398"/>
+      <c r="J32" s="398"/>
+      <c r="K32" s="398"/>
+      <c r="L32" s="399"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="371" t="s">
+      <c r="C33" s="387" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="372"/>
-      <c r="E33" s="372"/>
+      <c r="D33" s="388"/>
+      <c r="E33" s="388"/>
       <c r="F33" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="G33" s="373" t="s">
+      <c r="G33" s="389" t="s">
         <v>82</v>
       </c>
-      <c r="H33" s="384" t="s">
+      <c r="H33" s="400" t="s">
         <v>84</v>
       </c>
-      <c r="I33" s="385"/>
-      <c r="J33" s="385"/>
+      <c r="I33" s="401"/>
+      <c r="J33" s="401"/>
       <c r="K33" s="199" t="s">
         <v>83</v>
       </c>
-      <c r="L33" s="386" t="s">
+      <c r="L33" s="402" t="s">
         <v>82</v>
       </c>
     </row>
@@ -16253,7 +15403,7 @@
       <c r="F34" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="G34" s="374"/>
+      <c r="G34" s="390"/>
       <c r="H34" s="154" t="s">
         <v>81</v>
       </c>
@@ -16266,7 +15416,7 @@
       <c r="K34" s="151" t="s">
         <v>89</v>
       </c>
-      <c r="L34" s="386"/>
+      <c r="L34" s="402"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="142">
@@ -16342,16 +15492,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="L33:L34"/>
     <mergeCell ref="B4:H8"/>
     <mergeCell ref="E20:I20"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="M20:O20"/>
     <mergeCell ref="C32:G32"/>
     <mergeCell ref="H32:L32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="L33:L34"/>
   </mergeCells>
   <conditionalFormatting sqref="C35:L38">
     <cfRule type="containsBlanks" dxfId="117" priority="15">
@@ -16440,51 +15590,51 @@
       <c r="A4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
-      <c r="H4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="376"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
-      <c r="H5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
+      <c r="H5" s="376"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="76"/>
@@ -16609,23 +15759,23 @@
       <c r="B22" s="73"/>
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
-      <c r="E22" s="390" t="s">
+      <c r="E22" s="403" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="391"/>
-      <c r="G22" s="391"/>
-      <c r="H22" s="391"/>
-      <c r="I22" s="392"/>
-      <c r="J22" s="393" t="s">
+      <c r="F22" s="404"/>
+      <c r="G22" s="404"/>
+      <c r="H22" s="404"/>
+      <c r="I22" s="405"/>
+      <c r="J22" s="406" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="394"/>
-      <c r="L22" s="395"/>
-      <c r="M22" s="387" t="s">
+      <c r="K22" s="407"/>
+      <c r="L22" s="408"/>
+      <c r="M22" s="409" t="s">
         <v>70</v>
       </c>
-      <c r="N22" s="388"/>
-      <c r="O22" s="389"/>
+      <c r="N22" s="410"/>
+      <c r="O22" s="411"/>
     </row>
     <row r="23" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="80" t="s">
@@ -17083,45 +16233,45 @@
     </row>
     <row r="33" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C34" s="378" t="s">
+      <c r="C34" s="394" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="379"/>
-      <c r="E34" s="379"/>
-      <c r="F34" s="379"/>
-      <c r="G34" s="380"/>
-      <c r="H34" s="381" t="s">
+      <c r="D34" s="395"/>
+      <c r="E34" s="395"/>
+      <c r="F34" s="395"/>
+      <c r="G34" s="396"/>
+      <c r="H34" s="397" t="s">
         <v>70</v>
       </c>
-      <c r="I34" s="382"/>
-      <c r="J34" s="382"/>
-      <c r="K34" s="382"/>
-      <c r="L34" s="383"/>
+      <c r="I34" s="398"/>
+      <c r="J34" s="398"/>
+      <c r="K34" s="398"/>
+      <c r="L34" s="399"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="371" t="s">
+      <c r="C35" s="387" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="372"/>
-      <c r="E35" s="372"/>
+      <c r="D35" s="388"/>
+      <c r="E35" s="388"/>
       <c r="F35" s="200" t="s">
         <v>84</v>
       </c>
-      <c r="G35" s="373" t="s">
+      <c r="G35" s="389" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="384" t="s">
+      <c r="H35" s="400" t="s">
         <v>83</v>
       </c>
-      <c r="I35" s="385"/>
-      <c r="J35" s="385"/>
+      <c r="I35" s="401"/>
+      <c r="J35" s="401"/>
       <c r="K35" s="199" t="s">
         <v>84</v>
       </c>
-      <c r="L35" s="386" t="s">
+      <c r="L35" s="402" t="s">
         <v>82</v>
       </c>
     </row>
@@ -17141,7 +16291,7 @@
       <c r="F36" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="G36" s="374"/>
+      <c r="G36" s="390"/>
       <c r="H36" s="154" t="s">
         <v>81</v>
       </c>
@@ -17154,7 +16304,7 @@
       <c r="K36" s="151" t="s">
         <v>89</v>
       </c>
-      <c r="L36" s="386"/>
+      <c r="L36" s="402"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="142">
@@ -17230,16 +16380,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="L35:L36"/>
     <mergeCell ref="B4:H8"/>
     <mergeCell ref="E22:I22"/>
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="M22:O22"/>
     <mergeCell ref="C34:G34"/>
     <mergeCell ref="H34:L34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="L35:L36"/>
   </mergeCells>
   <conditionalFormatting sqref="C37:L40">
     <cfRule type="containsBlanks" dxfId="107" priority="15">
@@ -17328,51 +16478,51 @@
       <c r="A4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
-      <c r="H4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="376"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
-      <c r="H5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
+      <c r="H5" s="376"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="76"/>
@@ -17497,23 +16647,23 @@
       <c r="B22" s="73"/>
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
-      <c r="E22" s="390" t="s">
+      <c r="E22" s="403" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="391"/>
-      <c r="G22" s="391"/>
-      <c r="H22" s="391"/>
-      <c r="I22" s="392"/>
-      <c r="J22" s="393" t="s">
+      <c r="F22" s="404"/>
+      <c r="G22" s="404"/>
+      <c r="H22" s="404"/>
+      <c r="I22" s="405"/>
+      <c r="J22" s="406" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="394"/>
-      <c r="L22" s="395"/>
-      <c r="M22" s="387" t="s">
+      <c r="K22" s="407"/>
+      <c r="L22" s="408"/>
+      <c r="M22" s="409" t="s">
         <v>70</v>
       </c>
-      <c r="N22" s="388"/>
-      <c r="O22" s="389"/>
+      <c r="N22" s="410"/>
+      <c r="O22" s="411"/>
     </row>
     <row r="23" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="80" t="s">
@@ -17971,45 +17121,45 @@
     </row>
     <row r="33" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C34" s="378" t="s">
+      <c r="C34" s="394" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="379"/>
-      <c r="E34" s="379"/>
-      <c r="F34" s="379"/>
-      <c r="G34" s="380"/>
-      <c r="H34" s="381" t="s">
+      <c r="D34" s="395"/>
+      <c r="E34" s="395"/>
+      <c r="F34" s="395"/>
+      <c r="G34" s="396"/>
+      <c r="H34" s="397" t="s">
         <v>70</v>
       </c>
-      <c r="I34" s="382"/>
-      <c r="J34" s="382"/>
-      <c r="K34" s="382"/>
-      <c r="L34" s="383"/>
+      <c r="I34" s="398"/>
+      <c r="J34" s="398"/>
+      <c r="K34" s="398"/>
+      <c r="L34" s="399"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="371" t="s">
+      <c r="C35" s="387" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="372"/>
-      <c r="E35" s="372"/>
+      <c r="D35" s="388"/>
+      <c r="E35" s="388"/>
       <c r="F35" s="200" t="s">
         <v>83</v>
       </c>
-      <c r="G35" s="373" t="s">
+      <c r="G35" s="389" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="384" t="s">
+      <c r="H35" s="400" t="s">
         <v>84</v>
       </c>
-      <c r="I35" s="385"/>
-      <c r="J35" s="385"/>
+      <c r="I35" s="401"/>
+      <c r="J35" s="401"/>
       <c r="K35" s="199" t="s">
         <v>83</v>
       </c>
-      <c r="L35" s="386" t="s">
+      <c r="L35" s="402" t="s">
         <v>82</v>
       </c>
     </row>
@@ -18029,7 +17179,7 @@
       <c r="F36" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="G36" s="374"/>
+      <c r="G36" s="390"/>
       <c r="H36" s="154" t="s">
         <v>81</v>
       </c>
@@ -18042,7 +17192,7 @@
       <c r="K36" s="151" t="s">
         <v>89</v>
       </c>
-      <c r="L36" s="386"/>
+      <c r="L36" s="402"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="142">
@@ -18118,16 +17268,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="L35:L36"/>
     <mergeCell ref="B4:H8"/>
     <mergeCell ref="E22:I22"/>
     <mergeCell ref="J22:L22"/>
     <mergeCell ref="M22:O22"/>
     <mergeCell ref="C34:G34"/>
     <mergeCell ref="H34:L34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="L35:L36"/>
   </mergeCells>
   <conditionalFormatting sqref="C37:L40">
     <cfRule type="containsBlanks" dxfId="97" priority="15">
@@ -18218,51 +17368,51 @@
       <c r="A4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="360" t="s">
+      <c r="B4" s="376" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="360"/>
-      <c r="D4" s="360"/>
-      <c r="E4" s="360"/>
-      <c r="F4" s="360"/>
-      <c r="G4" s="360"/>
-      <c r="H4" s="360"/>
+      <c r="C4" s="376"/>
+      <c r="D4" s="376"/>
+      <c r="E4" s="376"/>
+      <c r="F4" s="376"/>
+      <c r="G4" s="376"/>
+      <c r="H4" s="376"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="360"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
-      <c r="G5" s="360"/>
-      <c r="H5" s="360"/>
+      <c r="B5" s="376"/>
+      <c r="C5" s="376"/>
+      <c r="D5" s="376"/>
+      <c r="E5" s="376"/>
+      <c r="F5" s="376"/>
+      <c r="G5" s="376"/>
+      <c r="H5" s="376"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="360"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
-      <c r="G6" s="360"/>
-      <c r="H6" s="360"/>
+      <c r="B6" s="376"/>
+      <c r="C6" s="376"/>
+      <c r="D6" s="376"/>
+      <c r="E6" s="376"/>
+      <c r="F6" s="376"/>
+      <c r="G6" s="376"/>
+      <c r="H6" s="376"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="360"/>
-      <c r="C7" s="360"/>
-      <c r="D7" s="360"/>
-      <c r="E7" s="360"/>
-      <c r="F7" s="360"/>
-      <c r="G7" s="360"/>
-      <c r="H7" s="360"/>
+      <c r="B7" s="376"/>
+      <c r="C7" s="376"/>
+      <c r="D7" s="376"/>
+      <c r="E7" s="376"/>
+      <c r="F7" s="376"/>
+      <c r="G7" s="376"/>
+      <c r="H7" s="376"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="360"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
-      <c r="G8" s="360"/>
-      <c r="H8" s="360"/>
+      <c r="B8" s="376"/>
+      <c r="C8" s="376"/>
+      <c r="D8" s="376"/>
+      <c r="E8" s="376"/>
+      <c r="F8" s="376"/>
+      <c r="G8" s="376"/>
+      <c r="H8" s="376"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="76"/>
@@ -18387,23 +17537,23 @@
       <c r="B22" s="73"/>
       <c r="C22" s="73"/>
       <c r="D22" s="73"/>
-      <c r="E22" s="390" t="s">
+      <c r="E22" s="403" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="391"/>
-      <c r="G22" s="391"/>
-      <c r="H22" s="391"/>
-      <c r="I22" s="392"/>
-      <c r="J22" s="393" t="s">
+      <c r="F22" s="404"/>
+      <c r="G22" s="404"/>
+      <c r="H22" s="404"/>
+      <c r="I22" s="405"/>
+      <c r="J22" s="406" t="s">
         <v>69</v>
       </c>
-      <c r="K22" s="394"/>
-      <c r="L22" s="395"/>
-      <c r="M22" s="387" t="s">
+      <c r="K22" s="407"/>
+      <c r="L22" s="408"/>
+      <c r="M22" s="409" t="s">
         <v>70</v>
       </c>
-      <c r="N22" s="388"/>
-      <c r="O22" s="389"/>
+      <c r="N22" s="410"/>
+      <c r="O22" s="411"/>
     </row>
     <row r="23" spans="1:17" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="80" t="s">
@@ -18861,53 +18011,53 @@
     </row>
     <row r="33" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="396" t="s">
+      <c r="C34" s="419" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="397"/>
-      <c r="E34" s="397"/>
-      <c r="F34" s="397"/>
-      <c r="G34" s="397"/>
-      <c r="H34" s="398"/>
-      <c r="I34" s="399" t="s">
+      <c r="D34" s="420"/>
+      <c r="E34" s="420"/>
+      <c r="F34" s="420"/>
+      <c r="G34" s="420"/>
+      <c r="H34" s="421"/>
+      <c r="I34" s="422" t="s">
         <v>70</v>
       </c>
-      <c r="J34" s="400"/>
-      <c r="K34" s="400"/>
-      <c r="L34" s="400"/>
-      <c r="M34" s="400"/>
-      <c r="N34" s="401"/>
+      <c r="J34" s="423"/>
+      <c r="K34" s="423"/>
+      <c r="L34" s="423"/>
+      <c r="M34" s="423"/>
+      <c r="N34" s="424"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="403" t="s">
+      <c r="C35" s="413" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="404"/>
-      <c r="E35" s="404"/>
+      <c r="D35" s="414"/>
+      <c r="E35" s="414"/>
       <c r="F35" s="205" t="s">
         <v>83</v>
       </c>
-      <c r="G35" s="404" t="s">
+      <c r="G35" s="414" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="405" t="s">
+      <c r="H35" s="415" t="s">
         <v>143</v>
       </c>
-      <c r="I35" s="407" t="s">
+      <c r="I35" s="417" t="s">
         <v>84</v>
       </c>
-      <c r="J35" s="408"/>
-      <c r="K35" s="408"/>
+      <c r="J35" s="418"/>
+      <c r="K35" s="418"/>
       <c r="L35" s="204" t="s">
         <v>83</v>
       </c>
-      <c r="M35" s="408" t="s">
+      <c r="M35" s="418" t="s">
         <v>82</v>
       </c>
-      <c r="N35" s="402" t="s">
+      <c r="N35" s="412" t="s">
         <v>143</v>
       </c>
     </row>
@@ -18927,8 +18077,8 @@
       <c r="F36" s="207" t="s">
         <v>89</v>
       </c>
-      <c r="G36" s="372"/>
-      <c r="H36" s="406"/>
+      <c r="G36" s="388"/>
+      <c r="H36" s="416"/>
       <c r="I36" s="154" t="s">
         <v>81</v>
       </c>
@@ -18941,8 +18091,8 @@
       <c r="L36" s="151" t="s">
         <v>89</v>
       </c>
-      <c r="M36" s="385"/>
-      <c r="N36" s="386"/>
+      <c r="M36" s="401"/>
+      <c r="N36" s="402"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="142">
@@ -19026,18 +18176,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B4:H8"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="I34:N34"/>
     <mergeCell ref="N35:N36"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="I35:K35"/>
     <mergeCell ref="M35:M36"/>
     <mergeCell ref="G35:G36"/>
-    <mergeCell ref="B4:H8"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="I34:N34"/>
   </mergeCells>
   <conditionalFormatting sqref="C37:E40 H37:H40">
     <cfRule type="containsBlanks" dxfId="87" priority="30">

</xml_diff>